<commit_message>
Created new sample data.
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -1,25 +1,53 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryder\Documents\Projects\EECE2140 Final Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D854C308-6060-4863-AFED-EBAF6D189FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>independant (s)</t>
+  </si>
+  <si>
+    <t>dependant (m)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +358,928 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="14.47265625" customWidth="1"/>
+    <col min="2" max="2" width="11.62890625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>5*EXP(A2/50)</f>
+        <v>5.1010067001337784</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B66" si="0">5*EXP(A3/50)</f>
+        <v>5.2040538709619408</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>5.3091827327267982</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>5.416435338374793</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>5.5258545903782386</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>5.6374842578968787</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>5.7513689942861372</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>5.8675543549590516</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>5.9860868156090508</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>6.1070137908008491</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>6.2303836529369043</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>6.3562457516070232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>6.4846504333288593</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>6.6156490616871846</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>6.7492940378800164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>6.8856388216797857</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>7.0247379528179685</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>7.1666470728017009</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>7.3114229471711223</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>7.4591234882063517</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>7.6098077780931686</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>7.7635360925566799</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>7.9203699249724089</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>8.0803720109644672</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>8.2436063535006419</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>8.410138248494432</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>8.580034310924292</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>8.7533625014805061</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>8.930192153750367</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>9.1105940019525438</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>9.2946402092317104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>9.4824043965247569</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>9.673961672010158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>9.8693886611522395</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>10.068763537352384</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>10.272166053219438</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>10.479677572471822</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>10.691381102484092</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>10.907361327491005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>11.127704642462339</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>11.352499187662028</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>11.581834883905458</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>11.815803468528973</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>12.054498532086049</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>12.298015555784749</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>12.54645194968149</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>12.799907091646357</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>13.058482367115589</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>13.322281209647084</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>13.591409142295225</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>13.865973819821489</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>14.146085071757799</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>14.431854946339794</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>14.723397755327621</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>15.020830119732167</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>15.324271016465012</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>15.633841825930777</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>15.949666380580922</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>16.271871014448354</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>16.600584613682734</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>16.935938668106672</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>17.278067323813378</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>17.627107436826911</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>17.983198627846409</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="0"/>
+        <v>18.34648333809622</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <f t="shared" ref="B67:B101" si="1">5*EXP(A67/50)</f>
+        <v>18.717106886304315</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="1"/>
+        <v>19.095217526831682</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="1"/>
+        <v>19.480966508976074</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="1"/>
+        <v>19.87450813747374</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="1"/>
+        <v>20.275999834223374</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="1"/>
+        <v>20.685602201256962</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="1"/>
+        <v>21.103479084982762</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="1"/>
+        <v>21.529797641726031</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="1"/>
+        <v>21.964728404593785</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="1"/>
+        <v>22.408445351690322</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="1"/>
+        <v>22.861125975710795</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="1"/>
+        <v>23.322951354940628</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="1"/>
+        <v>23.794106225689269</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="1"/>
+        <v>24.274779056187171</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="1"/>
+        <v>24.765162121975575</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="1"/>
+        <v>25.265451582819338</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="1"/>
+        <v>25.7758475611734</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="1"/>
+        <v>26.296554222234491</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="1"/>
+        <v>26.827779855609872</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="1"/>
+        <v>27.369736958636</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="1"/>
+        <v>27.92264232138027</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="1"/>
+        <v>28.486717113359955</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="1"/>
+        <v>29.062186972012945</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="1"/>
+        <v>29.64928209295573</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="1"/>
+        <v>30.248237322064732</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="1"/>
+        <v>30.85929224941777</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="1"/>
+        <v>31.482691305133287</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <f t="shared" si="1"/>
+        <v>32.118683857145676</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <f t="shared" si="1"/>
+        <v>32.767524310955743</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="1"/>
+        <v>33.429472211396345</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="1"/>
+        <v>34.104792346453749</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="1"/>
+        <v>34.793754853186357</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="1"/>
+        <v>35.49663532578316</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="1"/>
+        <v>36.213714925805064</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="1"/>
+        <v>36.945280494653254</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>